<commit_message>
03.02.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/January/All Details/30.01.2020/MC Balance Transfer Jan'2020.xlsx
+++ b/2020/January/All Details/30.01.2020/MC Balance Transfer Jan'2020.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Mugdho-Corporation\2020\January\All Details\30.01.2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Md. Naimul Haq\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76A668BA-BD35-43EB-B7D8-0B203421A44E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="0" windowWidth="13965" windowHeight="11070" tabRatio="598" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="0" windowWidth="13965" windowHeight="11070" tabRatio="598"/>
   </bookViews>
   <sheets>
     <sheet name="Oct'19 Sales+Cost+Bank+Balanch" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,12 +27,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>LENOVO</author>
   </authors>
   <commentList>
-    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{C14C18B4-A4EF-4D48-B6B8-C4603D1D9FE8}">
+    <comment ref="C37" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -62,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="98">
   <si>
     <t>Date</t>
   </si>
@@ -340,9 +339,6 @@
     <t>28.01.2020</t>
   </si>
   <si>
-    <t>Apurbo</t>
-  </si>
-  <si>
     <t>29.01.2020</t>
   </si>
   <si>
@@ -351,11 +347,20 @@
   <si>
     <t>L130*2</t>
   </si>
+  <si>
+    <t>30.01.2020</t>
+  </si>
+  <si>
+    <t>S.A Mobile</t>
+  </si>
+  <si>
+    <t>B.M Rahinul</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1219,7 +1224,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1354,23 +1359,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1406,23 +1394,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1598,14 +1569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="E43" sqref="E43"/>
     </sheetView>
@@ -3809,7 +3780,7 @@
     </row>
     <row r="29" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B29" s="2">
         <v>697495</v>
@@ -3833,7 +3804,7 @@
         <v>570</v>
       </c>
       <c r="J29" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K29" s="7"/>
       <c r="L29" s="19"/>
@@ -3888,21 +3859,33 @@
       <c r="BI29" s="7"/>
     </row>
     <row r="30" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="A30" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B30" s="2">
+        <v>361870</v>
+      </c>
+      <c r="C30" s="2">
+        <v>372311</v>
+      </c>
+      <c r="D30" s="2">
+        <v>630</v>
+      </c>
       <c r="E30" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>372941</v>
       </c>
       <c r="F30" s="94"/>
       <c r="G30" s="113"/>
       <c r="H30" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="96"/>
-      <c r="J30" s="95"/>
+      <c r="I30" s="96">
+        <v>920</v>
+      </c>
+      <c r="J30" s="95" t="s">
+        <v>95</v>
+      </c>
       <c r="K30" s="7"/>
       <c r="L30" s="19"/>
       <c r="M30" s="7"/>
@@ -4095,23 +4078,23 @@
       </c>
       <c r="B33" s="2">
         <f>SUM(B5:B32)</f>
-        <v>8607170</v>
+        <v>8969040</v>
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>8141068</v>
+        <v>8513379</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
-        <v>31268</v>
+        <v>31898</v>
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>8172336</v>
+        <v>8545277</v>
       </c>
       <c r="F33" s="94">
         <f>B33-E33</f>
-        <v>434834</v>
+        <v>423763</v>
       </c>
       <c r="G33" s="114"/>
       <c r="H33" s="124"/>
@@ -4385,7 +4368,7 @@
         <v>6870</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="134"/>
@@ -4456,7 +4439,7 @@
         <v>7000</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="94"/>
@@ -4598,7 +4581,7 @@
         <v>4000</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="134"/>
@@ -4659,10 +4642,16 @@
       <c r="BI40" s="7"/>
     </row>
     <row r="41" spans="1:61" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="40"/>
+      <c r="A41" s="40" t="s">
+        <v>97</v>
+      </c>
       <c r="B41" s="1"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="1"/>
+      <c r="C41" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="E41" s="20"/>
       <c r="F41" s="134"/>
       <c r="G41" s="116"/>
@@ -4868,7 +4857,7 @@
       <c r="A44" s="73"/>
       <c r="B44" s="74"/>
       <c r="C44" s="75">
-        <v>0</v>
+        <v>6324</v>
       </c>
       <c r="D44" s="76"/>
       <c r="E44" s="3"/>
@@ -5135,7 +5124,6 @@
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
       <c r="H48" s="12"/>
       <c r="I48" s="64"/>
       <c r="J48" s="77"/>
@@ -5259,7 +5247,7 @@
         <v>98510</v>
       </c>
       <c r="D50" s="102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="12"/>
@@ -5323,10 +5311,10 @@
       </c>
       <c r="B51" s="43"/>
       <c r="C51" s="98">
-        <v>537680</v>
+        <v>497680</v>
       </c>
       <c r="D51" s="99" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="43"/>
@@ -5395,7 +5383,7 @@
         <v>198600</v>
       </c>
       <c r="D52" s="102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="12"/>
@@ -5533,7 +5521,7 @@
         <v>38000</v>
       </c>
       <c r="D54" s="102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="12"/>
@@ -5664,10 +5652,10 @@
       </c>
       <c r="B56" s="43"/>
       <c r="C56" s="98">
-        <v>170000</v>
+        <v>160000</v>
       </c>
       <c r="D56" s="97" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="43"/>
@@ -5799,7 +5787,7 @@
         <v>6000</v>
       </c>
       <c r="D58" s="107" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="64"/>
@@ -5861,14 +5849,14 @@
     </row>
     <row r="59" spans="1:61" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="100" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B59" s="43"/>
       <c r="C59" s="98">
         <v>4000</v>
       </c>
       <c r="D59" s="107" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="43"/>
@@ -5934,10 +5922,10 @@
       </c>
       <c r="B60" s="43"/>
       <c r="C60" s="98">
-        <v>56150</v>
+        <v>87755</v>
       </c>
       <c r="D60" s="99" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="43"/>
@@ -6067,17 +6055,11 @@
       <c r="BI61" s="7"/>
     </row>
     <row r="62" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="100" t="s">
-        <v>92</v>
-      </c>
+      <c r="A62" s="100"/>
       <c r="B62" s="43"/>
-      <c r="C62" s="98">
-        <v>5000</v>
-      </c>
-      <c r="D62" s="99" t="s">
-        <v>91</v>
-      </c>
-      <c r="E62" s="3"/>
+      <c r="C62" s="98"/>
+      <c r="D62" s="99"/>
+      <c r="E62" s="12"/>
       <c r="F62" s="155" t="s">
         <v>26</v>
       </c>
@@ -6149,7 +6131,7 @@
       </c>
       <c r="B63" s="43"/>
       <c r="C63" s="98">
-        <v>107000</v>
+        <v>100000</v>
       </c>
       <c r="D63" s="99" t="s">
         <v>90</v>
@@ -6220,7 +6202,7 @@
         <v>78</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C64" s="98">
         <v>2140</v>
@@ -6290,10 +6272,16 @@
       <c r="BI64" s="7"/>
     </row>
     <row r="65" spans="1:61" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="100"/>
+      <c r="A65" s="100" t="s">
+        <v>96</v>
+      </c>
       <c r="B65" s="43"/>
-      <c r="C65" s="98"/>
-      <c r="D65" s="99"/>
+      <c r="C65" s="98">
+        <v>10000</v>
+      </c>
+      <c r="D65" s="99" t="s">
+        <v>95</v>
+      </c>
       <c r="E65" s="3"/>
       <c r="F65" s="24"/>
       <c r="G65" s="13" t="s">
@@ -8654,7 +8642,7 @@
       <c r="B98" s="154"/>
       <c r="C98" s="45">
         <f>SUM(C37:C97)</f>
-        <v>1913044</v>
+        <v>1901973</v>
       </c>
       <c r="D98" s="41"/>
       <c r="F98" s="23"/>
@@ -8789,7 +8777,7 @@
       <c r="B100" s="152"/>
       <c r="C100" s="42">
         <f>C98+L121</f>
-        <v>1913044</v>
+        <v>1901973</v>
       </c>
       <c r="D100" s="26"/>
       <c r="F100" s="24"/>

</xml_diff>